<commit_message>
Add wl to parameter range compilation and perform inversions with 3 sets of priors
</commit_message>
<xml_diff>
--- a/data/paramcompilation.xlsx
+++ b/data/paramcompilation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/particle/Drive/ucsc/code/pyrite-dev/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD96266-5528-6849-A8E0-4F85D548DB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19825B23-2CA6-EF4A-9851-531223F4EA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="2040" windowWidth="27320" windowHeight="14860" activeTab="2" xr2:uid="{CA0E59E6-A1B0-4140-AD7C-5A6E20CF7AD2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="B2" sheetId="1" r:id="rId1"/>
     <sheet name="Bm2" sheetId="2" r:id="rId2"/>
     <sheet name="Bm1" sheetId="3" r:id="rId3"/>
+    <sheet name="wl" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="11">
   <si>
     <t>MNA</t>
   </si>
@@ -59,12 +60,24 @@
   <si>
     <t>id</t>
   </si>
+  <si>
+    <t>MBATS</t>
+  </si>
+  <si>
+    <t>MSARG</t>
+  </si>
+  <si>
+    <t>MWAP1</t>
+  </si>
+  <si>
+    <t>MWAP2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,6 +88,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1065,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA8465D-C0A6-7049-8515-6AE45AB8922D}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1430,4 +1449,620 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED29151-01E4-1241-9198-D6CA55B87B52}">
+  <dimension ref="A1:B75"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9.74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>29.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>54.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>8.83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>8.7200000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>7.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>9.9600000000000009</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>9.58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>5.23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>5.12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>7.97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55">
+        <v>78.787878800000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56">
+        <v>24.242424199999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57">
+        <v>22.222222200000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58">
+        <v>30.3030303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59">
+        <v>47.474747499999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>53.535353499999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>143.43434300000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62">
+        <v>66.666666699999993</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63">
+        <v>38.383838400000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64">
+        <v>35.353535399999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65">
+        <v>73.737373700000006</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>80.808080799999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67">
+        <v>91.919191900000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68">
+        <v>57.575757600000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69">
+        <v>38.383838400000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70">
+        <v>45.454545500000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71">
+        <v>72.7272727</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B72">
+        <v>76.767676800000004</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73">
+        <v>149.49494899999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74">
+        <v>87.878787900000006</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>44.444444400000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the spreadsheet (not included in last commit)
</commit_message>
<xml_diff>
--- a/data/paramcompilation.xlsx
+++ b/data/paramcompilation.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/particle/Drive/ucsc/code/pyrite-dev/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB399F3-A0F1-1540-ABD0-2E18EA494BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839CC0F5-4086-D845-84AE-F4BCC5056D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="2040" windowWidth="27320" windowHeight="14860" activeTab="4" xr2:uid="{CA0E59E6-A1B0-4140-AD7C-5A6E20CF7AD2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" activeTab="3" xr2:uid="{CA0E59E6-A1B0-4140-AD7C-5A6E20CF7AD2}"/>
   </bookViews>
   <sheets>
     <sheet name="B2" sheetId="1" r:id="rId1"/>
     <sheet name="Bm2" sheetId="2" r:id="rId2"/>
-    <sheet name="Bm1" sheetId="3" r:id="rId3"/>
-    <sheet name="wl" sheetId="6" r:id="rId4"/>
-    <sheet name="ws" sheetId="7" r:id="rId5"/>
+    <sheet name="Bm1s" sheetId="3" r:id="rId3"/>
+    <sheet name="Bm1l" sheetId="8" r:id="rId4"/>
+    <sheet name="wl" sheetId="6" r:id="rId5"/>
+    <sheet name="ws" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="23">
   <si>
     <t>MNA</t>
   </si>
@@ -99,6 +100,15 @@
   </si>
   <si>
     <t>V08</t>
+  </si>
+  <si>
+    <t>ENA</t>
+  </si>
+  <si>
+    <t>ENP</t>
+  </si>
+  <si>
+    <t>SBB</t>
   </si>
 </sst>
 </file>
@@ -1480,6 +1490,141 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44E551E-0D79-4848-B208-5071FF417B9A}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>1.21E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>2.3199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>2.4299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>4.0899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>3.7400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>5.6599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>3.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>4.2299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>9.8199999999999996E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>7.85E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0.27879999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0.73070000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>0.63080000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED29151-01E4-1241-9198-D6CA55B87B52}">
   <dimension ref="A1:B734"/>
   <sheetViews>
@@ -7370,11 +7515,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7445314A-0DC6-4B44-BABE-238FDC9EBCD2}">
   <dimension ref="A1:B692"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>